<commit_message>
Ya puedo agarrar la primera fila del excel y obtener todos los resultados siguientes de 1 columna especifica
</commit_message>
<xml_diff>
--- a/SAI/public/registroPago/registroPago1.xlsx
+++ b/SAI/public/registroPago/registroPago1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>fecha pagado</t>
   </si>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -132,7 +132,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -493,15 +493,102 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2">
+        <v>43260</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B2*1.5</f>
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2">
+        <v>43260</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B5" si="0">B3*1.5</f>
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2">
+        <v>43260</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>337.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H5">
       <formula1>datos!$A$2:$A$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>datos!$C$2:$C$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
       <formula1>datos!$B$2:$B$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Ya registra el pago en la base de datos correctamente desde un archivo de excelgit status!    NO TIENE VALIDACIONES, unicamente un script que verificael tipo de archivo xlsx
</commit_message>
<xml_diff>
--- a/SAI/public/registroPago/registroPago1.xlsx
+++ b/SAI/public/registroPago/registroPago1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>fecha pagado</t>
   </si>
@@ -431,7 +431,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -478,10 +478,10 @@
         <v>43260</v>
       </c>
       <c r="B2" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -489,96 +489,27 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
       <c r="I2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2">
-        <v>43260</v>
-      </c>
-      <c r="B3" s="3">
-        <f>B2*1.5</f>
-        <v>150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2">
-        <v>43260</v>
-      </c>
-      <c r="B4" s="3">
-        <f t="shared" ref="B4:B5" si="0">B3*1.5</f>
-        <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2">
-        <v>43260</v>
-      </c>
-      <c r="B5" s="3">
-        <f t="shared" si="0"/>
-        <v>337.5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>